<commit_message>
Todos los formularios completos.
</commit_message>
<xml_diff>
--- a/documentos/Tareas.xlsx
+++ b/documentos/Tareas.xlsx
@@ -58,6 +58,7 @@
         <sz val="12"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">&gt;&gt; </t>
     </r>
@@ -66,6 +67,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Ver Contratista / Servicios Profesionales</t>
     </r>
@@ -234,11 +236,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -260,40 +263,53 @@
       <sz val="12"/>
       <name val="tahoma;sans-serif"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="tahoma;sans-serif"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="tahoma;sans-serif"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFC9211E"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -500,88 +516,88 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" guid="{ABA370F8-6657-4DEF-845C-98A76BADDF14}">
-  <header guid="{C18515F4-28CF-4C7C-83C1-9F35F5EA1BB4}" dateTime="2020-12-20T12:33:00.000000000Z" userName=" " r:id="rId1" minRId="1" maxRId="2" maxSheetId="2">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" guid="{AB9FA9CD-4179-4495-BB0F-1671E9CFDCD4}">
+  <header guid="{BF019AF9-5B36-4625-A7FB-5442DCB288B0}" dateTime="2020-12-20T12:33:00.000000000Z" userName=" " r:id="rId1" minRId="1" maxRId="2" maxSheetId="2">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
   </header>
-  <header guid="{00C32530-0456-4E24-9D1B-BEE8B4198169}" dateTime="2020-12-20T12:34:00.000000000Z" userName=" " r:id="rId2" minRId="3" maxRId="3" maxSheetId="2">
+  <header guid="{8E510420-DCEC-4C3E-A84F-419DD26C96E3}" dateTime="2020-12-20T14:43:00.000000000Z" userName=" " r:id="rId2" minRId="3" maxRId="4" maxSheetId="2">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
   </header>
-  <header guid="{7E86B1C9-E907-4620-8ECC-C8FD3845C022}" dateTime="2020-12-20T13:11:00.000000000Z" userName=" " r:id="rId3" minRId="4" maxRId="4" maxSheetId="2">
+  <header guid="{B35A07A3-7107-4657-8E17-82552F7EB4E9}" dateTime="2020-12-20T14:44:00.000000000Z" userName=" " r:id="rId3" minRId="5" maxRId="6" maxSheetId="2">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
   </header>
-  <header guid="{3F0F620F-3413-49C1-BD26-C5ECDC9D041C}" dateTime="2020-12-20T14:32:00.000000000Z" userName=" " r:id="rId4" minRId="5" maxRId="6" maxSheetId="2">
+  <header guid="{E408092A-45FC-4149-9BAE-8991246CA9F6}" dateTime="2020-12-20T14:49:00.000000000Z" userName=" " r:id="rId4" minRId="7" maxRId="7" maxSheetId="2">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
   </header>
-  <header guid="{D0E98D5C-F13A-4FC1-BCEE-8A4EFCC94EDF}" dateTime="2020-12-20T14:36:00.000000000Z" userName=" " r:id="rId5" minRId="7" maxRId="7" maxSheetId="2">
+  <header guid="{CEBE9FA7-9892-465D-AD1D-18DD2395170F}" dateTime="2020-12-20T14:50:00.000000000Z" userName=" " r:id="rId5" minRId="8" maxRId="11" maxSheetId="2">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
   </header>
-  <header guid="{29883B45-0B03-4E10-B171-E1BDAF841B2C}" dateTime="2020-12-20T14:37:00.000000000Z" userName=" " r:id="rId6" minRId="8" maxRId="9" maxSheetId="2">
+  <header guid="{B4C12D50-278D-459D-A8A0-90CE8CFCDF44}" dateTime="2020-12-20T15:01:00.000000000Z" userName=" " r:id="rId6" minRId="12" maxRId="17" maxSheetId="2">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
   </header>
-  <header guid="{1F6F05A9-C159-4EEF-A64F-D8056BC50EDB}" dateTime="2020-12-20T14:38:00.000000000Z" userName=" " r:id="rId7" minRId="10" maxRId="10" maxSheetId="2">
+  <header guid="{7B980977-407C-4315-9608-51F8624A6AB3}" dateTime="2020-12-20T15:03:00.000000000Z" userName=" " r:id="rId7" minRId="18" maxRId="18" maxSheetId="2">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
   </header>
-  <header guid="{1D7BFC64-0187-41AF-BB33-693FFCB90CA0}" dateTime="2020-12-20T14:39:00.000000000Z" userName=" " r:id="rId8" minRId="11" maxRId="12" maxSheetId="2">
+  <header guid="{05ACF250-B132-4237-9D85-7CEDB63A5883}" dateTime="2020-12-20T15:11:00.000000000Z" userName=" " r:id="rId8" minRId="19" maxRId="20" maxSheetId="2">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
   </header>
-  <header guid="{2CEBE2EF-FD47-44E8-8BBA-FD7A0FC86111}" dateTime="2020-12-20T14:40:00.000000000Z" userName=" " r:id="rId9" minRId="13" maxRId="13" maxSheetId="2">
+  <header guid="{86DBD2D5-1AF7-47F7-93C2-CA0FCCE990D5}" dateTime="2020-12-21T18:58:00.000000000Z" userName=" " r:id="rId9" minRId="21" maxRId="21" maxSheetId="2">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
   </header>
-  <header guid="{9CF3CE75-77D9-4F1B-BD9C-AE3ADBE0AC41}" dateTime="2020-12-20T14:43:00.000000000Z" userName=" " r:id="rId10" minRId="14" maxRId="15" maxSheetId="2">
+  <header guid="{71050611-0847-44B0-AB55-8A298C0F08FE}" dateTime="2020-12-20T12:34:00.000000000Z" userName=" " r:id="rId10" minRId="22" maxRId="22" maxSheetId="2">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
   </header>
-  <header guid="{3B79746F-A28A-41FE-95C8-5DE99B624422}" dateTime="2020-12-20T14:44:00.000000000Z" userName=" " r:id="rId11" minRId="16" maxRId="17" maxSheetId="2">
+  <header guid="{EB9B4BEE-7B18-424C-B61D-86F45A7C7626}" dateTime="2020-12-20T13:11:00.000000000Z" userName=" " r:id="rId11" minRId="23" maxRId="23" maxSheetId="2">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
   </header>
-  <header guid="{BFD8C11B-918C-49DB-ADC1-371872A76352}" dateTime="2020-12-20T14:49:00.000000000Z" userName=" " r:id="rId12" minRId="18" maxRId="18" maxSheetId="2">
+  <header guid="{B6127B26-2ACB-4EC1-BC9E-F872E55B54FE}" dateTime="2020-12-20T14:32:00.000000000Z" userName=" " r:id="rId12" minRId="24" maxRId="25" maxSheetId="2">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
   </header>
-  <header guid="{C5528949-F6F2-4F97-8732-83C7EE74578D}" dateTime="2020-12-20T14:50:00.000000000Z" userName=" " r:id="rId13" minRId="19" maxRId="22" maxSheetId="2">
+  <header guid="{FA3E3F01-A509-4E51-A8B6-60DA76577D52}" dateTime="2020-12-20T14:36:00.000000000Z" userName=" " r:id="rId13" minRId="26" maxRId="26" maxSheetId="2">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
   </header>
-  <header guid="{75CF825E-9BCB-4805-9F6C-E706E26692FF}" dateTime="2020-12-20T15:01:00.000000000Z" userName=" " r:id="rId14" minRId="23" maxRId="28" maxSheetId="2">
+  <header guid="{F6D84013-22B1-4B04-BD81-5CA4A8962384}" dateTime="2020-12-20T14:37:00.000000000Z" userName=" " r:id="rId14" minRId="27" maxRId="28" maxSheetId="2">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
   </header>
-  <header guid="{E5ECC8DE-14C7-46A4-AE01-1A5D9EF601E4}" dateTime="2020-12-20T15:03:00.000000000Z" userName=" " r:id="rId15" minRId="29" maxRId="29" maxSheetId="2">
+  <header guid="{A9714F04-CB45-49AD-8B1C-BCFDA24954B4}" dateTime="2020-12-20T14:38:00.000000000Z" userName=" " r:id="rId15" minRId="29" maxRId="29" maxSheetId="2">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
   </header>
-  <header guid="{F5BEF53E-F24B-45BB-A4EE-FCFFEFC4FA36}" dateTime="2020-12-20T15:11:00.000000000Z" userName=" " r:id="rId16" minRId="30" maxRId="31" maxSheetId="2">
+  <header guid="{A37D518D-D920-4F2E-834A-AE874A095DC7}" dateTime="2020-12-20T14:39:00.000000000Z" userName=" " r:id="rId16" minRId="30" maxRId="31" maxSheetId="2">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
   </header>
-  <header guid="{ABA370F8-6657-4DEF-845C-98A76BADDF14}" dateTime="2020-12-21T18:58:00.000000000Z" userName=" " r:id="rId17" minRId="32" maxRId="32" maxSheetId="2">
+  <header guid="{AB9FA9CD-4179-4495-BB0F-1671E9CFDCD4}" dateTime="2020-12-20T14:40:00.000000000Z" userName=" " r:id="rId17" minRId="32" maxRId="32" maxSheetId="2">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
@@ -596,9 +612,10 @@
       <is>
         <r>
           <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Como en los casos anteriores, estos procedmiiento implican una remaquitacion de los formularios porque se pensaron en fucniòn de los formularios enviados</t>
         </r>
@@ -618,21 +635,142 @@
 
 <file path=xl/revisions/revisionLog10.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="14" ua="false" sId="1">
+  <rcc rId="22" ua="false" sId="1">
+    <nc r="D36" t="n">
+      <v>0</v>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog11.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="23" ua="false" sId="1">
+    <nc r="E27" t="inlineStr">
+      <is>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Trae el formualrio original. Recomiendo dejarlo así.</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog12.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="24" ua="false" sId="1">
+    <oc r="D32" t="n">
+      <v>1</v>
+    </oc>
+    <nc r="D32" t="n">
+      <v>0.3</v>
+    </nc>
+  </rcc>
+  <rcc rId="25" ua="false" sId="1">
+    <nc r="D35" t="n">
+      <v>2</v>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog13.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="26" ua="false" sId="1">
+    <nc r="D7" t="n">
+      <v>0</v>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog14.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="27" ua="false" sId="1">
+    <nc r="D52" t="n">
+      <v>8</v>
+    </nc>
+  </rcc>
+  <rcc rId="28" ua="false" sId="1">
+    <nc r="D57" t="n">
+      <v>8</v>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog15.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="29" ua="false" sId="1">
+    <oc r="D28" t="n">
+      <v>1</v>
+    </oc>
+    <nc r="D28" t="n">
+      <v>1.5</v>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog16.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="30" ua="false" sId="1">
+    <oc r="D29" t="n">
+      <v>0.2</v>
+    </oc>
+    <nc r="D29" t="n">
+      <v>0.3</v>
+    </nc>
+  </rcc>
+  <rcc rId="31" ua="false" sId="1">
+    <oc r="D35" t="n">
+      <v>2</v>
+    </oc>
+    <nc r="D35" t="n">
+      <v>3</v>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog17.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="32" ua="false" sId="1">
+    <oc r="D28" t="n">
+      <v>1.5</v>
+    </oc>
+    <nc r="D28" t="n">
+      <v>2</v>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="3" ua="false" sId="1">
     <nc r="E28" t="inlineStr">
       <is>
         <r>
           <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">En caso de hacer un menu desplegable y que el usuario requiera colocar mas de una provincia, hay que desarrollar una tabla extra relacionada con el proveedor donde figuren las provincias elegidas.</t>
         </r>
       </is>
     </nc>
   </rcc>
-  <rcc rId="15" ua="false" sId="1">
+  <rcc rId="4" ua="false" sId="1">
     <oc r="D27" t="n">
       <v>3</v>
     </oc>
@@ -643,9 +781,9 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/revisionLog11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/revisionLog3.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="16" ua="false" sId="1">
+  <rcc rId="5" ua="false" sId="1">
     <oc r="D28" t="n">
       <v>2</v>
     </oc>
@@ -653,7 +791,7 @@
       <v>5</v>
     </nc>
   </rcc>
-  <rcc rId="17" ua="false" sId="1">
+  <rcc rId="6" ua="false" sId="1">
     <nc r="D37" t="n">
       <v>0</v>
     </nc>
@@ -661,9 +799,9 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/revisionLog12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/revisionLog4.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="18" ua="false" sId="1">
+  <rcc rId="7" ua="false" sId="1">
     <oc r="D30" t="n">
       <v>3</v>
     </oc>
@@ -674,9 +812,9 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/revisionLog13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/revisionLog5.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="19" ua="false" sId="1">
+  <rcc rId="8" ua="false" sId="1">
     <oc r="D28" t="n">
       <v>5</v>
     </oc>
@@ -684,7 +822,7 @@
       <v>7</v>
     </nc>
   </rcc>
-  <rcc rId="20" ua="false" sId="1">
+  <rcc rId="9" ua="false" sId="1">
     <oc r="D44" t="n">
       <v>8</v>
     </oc>
@@ -692,7 +830,7 @@
       <v>10</v>
     </nc>
   </rcc>
-  <rcc rId="21" ua="false" sId="1">
+  <rcc rId="10" ua="false" sId="1">
     <oc r="D52" t="n">
       <v>8</v>
     </oc>
@@ -700,7 +838,7 @@
       <v>10</v>
     </nc>
   </rcc>
-  <rcc rId="22" ua="false" sId="1">
+  <rcc rId="11" ua="false" sId="1">
     <oc r="D57" t="n">
       <v>8</v>
     </oc>
@@ -711,9 +849,9 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/revisionLog14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/revisionLog6.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="23" ua="false" sId="1">
+  <rcc rId="12" ua="false" sId="1">
     <oc r="D6" t="n">
       <v>0</v>
     </oc>
@@ -721,7 +859,7 @@
       <v>0.1</v>
     </nc>
   </rcc>
-  <rcc rId="24" ua="false" sId="1">
+  <rcc rId="13" ua="false" sId="1">
     <oc r="D7" t="n">
       <v>0</v>
     </oc>
@@ -729,7 +867,7 @@
       <v>0.1</v>
     </nc>
   </rcc>
-  <rcc rId="25" ua="false" sId="1">
+  <rcc rId="14" ua="false" sId="1">
     <oc r="D9" t="n">
       <v>0</v>
     </oc>
@@ -737,21 +875,22 @@
       <v>0.1</v>
     </nc>
   </rcc>
-  <rcc rId="26" ua="false" sId="1">
+  <rcc rId="15" ua="false" sId="1">
     <nc r="E9" t="inlineStr">
       <is>
         <r>
           <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">sin la carga de subrubros desde el excel</t>
         </r>
       </is>
     </nc>
   </rcc>
-  <rcc rId="27" ua="false" sId="1">
+  <rcc rId="16" ua="false" sId="1">
     <oc r="D10" t="n">
       <v>0</v>
     </oc>
@@ -759,7 +898,7 @@
       <v>0.1</v>
     </nc>
   </rcc>
-  <rcc rId="28" ua="false" sId="1">
+  <rcc rId="17" ua="false" sId="1">
     <oc r="D17" t="n">
       <v>1</v>
     </oc>
@@ -770,16 +909,17 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/revisionLog15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/revisionLog7.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="29" ua="false" sId="1">
+  <rcc rId="18" ua="false" sId="1">
     <nc r="E18" t="inlineStr">
       <is>
         <r>
           <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Es necesario?</t>
         </r>
@@ -789,9 +929,9 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/revisionLog16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/revisionLog8.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="30" ua="false" sId="1">
+  <rcc rId="19" ua="false" sId="1">
     <oc r="D18" t="n">
       <v>1.2</v>
     </oc>
@@ -799,14 +939,15 @@
       <v>2.5</v>
     </nc>
   </rcc>
-  <rcc rId="31" ua="false" sId="1">
+  <rcc rId="20" ua="false" sId="1">
     <oc r="E18" t="inlineStr">
       <is>
         <r>
           <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="0"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Es necesario?</t>
         </r>
@@ -817,133 +958,14 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/revisionLog17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/revisionLog9.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="32" ua="false" sId="1">
+  <rcc rId="21" ua="false" sId="1">
     <oc r="D19" t="n">
       <v>5</v>
     </oc>
     <nc r="D19" t="n">
       <v>0</v>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="3" ua="false" sId="1">
-    <nc r="D36" t="n">
-      <v>0</v>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog3.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="4" ua="false" sId="1">
-    <nc r="E27" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Trae el formualrio original. Recomiendo dejarlo así.</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog4.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="5" ua="false" sId="1">
-    <oc r="D32" t="n">
-      <v>1</v>
-    </oc>
-    <nc r="D32" t="n">
-      <v>0.3</v>
-    </nc>
-  </rcc>
-  <rcc rId="6" ua="false" sId="1">
-    <nc r="D35" t="n">
-      <v>2</v>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog5.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="7" ua="false" sId="1">
-    <nc r="D7" t="n">
-      <v>0</v>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog6.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="8" ua="false" sId="1">
-    <nc r="D52" t="n">
-      <v>8</v>
-    </nc>
-  </rcc>
-  <rcc rId="9" ua="false" sId="1">
-    <nc r="D57" t="n">
-      <v>8</v>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog7.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="10" ua="false" sId="1">
-    <oc r="D28" t="n">
-      <v>1</v>
-    </oc>
-    <nc r="D28" t="n">
-      <v>1.5</v>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog8.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="11" ua="false" sId="1">
-    <oc r="D29" t="n">
-      <v>0.2</v>
-    </oc>
-    <nc r="D29" t="n">
-      <v>0.3</v>
-    </nc>
-  </rcc>
-  <rcc rId="12" ua="false" sId="1">
-    <oc r="D35" t="n">
-      <v>2</v>
-    </oc>
-    <nc r="D35" t="n">
-      <v>3</v>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog9.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <rcc rId="13" ua="false" sId="1">
-    <oc r="D28" t="n">
-      <v>1.5</v>
-    </oc>
-    <nc r="D28" t="n">
-      <v>2</v>
     </nc>
   </rcc>
 </revisions>
@@ -960,11 +982,11 @@
   </sheetPr>
   <dimension ref="A1:BL63"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A37" activeCellId="0" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="125.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="43.2"/>
@@ -2980,11 +3002,11 @@
       <c r="BK36" s="4"/>
       <c r="BL36" s="4"/>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="2" t="s">
+    <row r="37" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D37" s="0" t="n">
+      <c r="D37" s="3" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>